<commit_message>
HW: PS1-1: Capacitors added to ADC input signals as anti-aliassing filter, GND_PWR net added, varistor replaced with gas discharge tube (GDT), high-voltage resistors adjusted to availability, netclasses extended, GPIO pinout assigned, tag-connect swapped for double-sided variant, routing completed, no DRC errors
</commit_message>
<xml_diff>
--- a/hw/PS1-1/Admin/STM32G474 pinout.xlsx
+++ b/hw/PS1-1/Admin/STM32G474 pinout.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\bat_source\hw\PS1-1\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E4F842-6F21-4F20-B49D-1EFB6F82A902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA2C907-AFF7-45EF-B6EA-919F1803E820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="2" xr2:uid="{21A4FC59-0757-4566-8791-AF29D3D9F0F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="3" xr2:uid="{21A4FC59-0757-4566-8791-AF29D3D9F0F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="3" r:id="rId1"/>
     <sheet name="Timer" sheetId="1" r:id="rId2"/>
-    <sheet name="ADC" sheetId="2" r:id="rId3"/>
-    <sheet name="Restricted GPIOs" sheetId="4" r:id="rId4"/>
-    <sheet name="GPIOs QFP100" sheetId="5" r:id="rId5"/>
+    <sheet name="UART" sheetId="6" r:id="rId3"/>
+    <sheet name="ADC" sheetId="2" r:id="rId4"/>
+    <sheet name="Restricted GPIOs" sheetId="4" r:id="rId5"/>
+    <sheet name="GPIOs QFP100" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="280">
   <si>
     <t>Timer overview</t>
   </si>
@@ -862,6 +862,51 @@
   </si>
   <si>
     <t>shared with ADC2</t>
+  </si>
+  <si>
+    <t>UART3</t>
+  </si>
+  <si>
+    <t>UART4</t>
+  </si>
+  <si>
+    <t>UART5</t>
+  </si>
+  <si>
+    <t>Available RX</t>
+  </si>
+  <si>
+    <t>UART Module</t>
+  </si>
+  <si>
+    <t>Available TX</t>
+  </si>
+  <si>
+    <t>Blocked by SPI</t>
+  </si>
+  <si>
+    <t>PB8</t>
+  </si>
+  <si>
+    <t>USART2</t>
+  </si>
+  <si>
+    <t>PD6, (PB4)</t>
+  </si>
+  <si>
+    <t>PC5, PE1, (PB7)</t>
+  </si>
+  <si>
+    <t>USART1</t>
+  </si>
+  <si>
+    <t>PC4, PE0, (PB6)</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>Pin changed during layouting</t>
   </si>
 </sst>
 </file>
@@ -891,12 +936,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -926,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -934,6 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2273,11 +2325,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCBC468-5DCA-4C9B-A202-E607297D0B02}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AE1967-F282-4108-9A8D-678FB35305D6}">
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,15 +2438,15 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2880,15 +3018,15 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -2983,7 +3121,10 @@
         <v>4</v>
       </c>
       <c r="L26" s="4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="M26" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3573,7 +3714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B98EFC0-842C-4E2C-9ADD-C61BC67F662B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -3815,7 +3956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7680DADC-115D-4B61-ADB4-956569A4F367}">
   <dimension ref="A1:D101"/>
   <sheetViews>

</xml_diff>